<commit_message>
progress bar working.. mostly
</commit_message>
<xml_diff>
--- a/data/inputs/Asset Model - Pole - Demo.xlsx
+++ b/data/inputs/Asset Model - Pole - Demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtreseder\OneDrive - KPMG\Documents\3. Client\Essential Energy\Probability of Failure Model\pof\data\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2079" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{90852C7C-C5C5-4CB8-8C7D-3CAF1C74C535}"/>
+  <xr:revisionPtr revIDLastSave="2084" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FCB75139-2875-4347-A496-BF1D5E822264}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="321">
   <si>
     <t>Cause</t>
   </si>
@@ -359,304 +359,307 @@
     <t>as_bad_as_old</t>
   </si>
   <si>
+    <t>groundline</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>ssf_calc</t>
+  </si>
+  <si>
+    <t>lean_angle</t>
+  </si>
+  <si>
+    <t>termite_powder</t>
+  </si>
+  <si>
+    <t>repair</t>
+  </si>
+  <si>
+    <t>ConditionTask</t>
+  </si>
+  <si>
+    <t>grp</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>reduction_factor</t>
+  </si>
+  <si>
+    <t>CAT3/4 replacement</t>
+  </si>
+  <si>
+    <t>replace</t>
+  </si>
+  <si>
+    <t>as_good_as_new</t>
+  </si>
+  <si>
+    <t>emergency replacement</t>
+  </si>
+  <si>
+    <t>fungal decay _ internal</t>
+  </si>
+  <si>
+    <t>CAT1/2 replacement</t>
+  </si>
+  <si>
+    <t>lightning</t>
+  </si>
+  <si>
+    <t>step</t>
+  </si>
+  <si>
+    <t>protection_inspection</t>
+  </si>
+  <si>
+    <t>protection</t>
+  </si>
+  <si>
+    <t>leaning</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>Sub System</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Maintainable Item</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>Pole</t>
+  </si>
+  <si>
+    <t>Pole Stay</t>
+  </si>
+  <si>
+    <t>Pole Cap</t>
+  </si>
+  <si>
+    <t>Pole Footing</t>
+  </si>
+  <si>
+    <t>pole (common)</t>
+  </si>
+  <si>
+    <t>pole (timber)</t>
+  </si>
+  <si>
+    <t>pole (concrete)</t>
+  </si>
+  <si>
+    <t>pole (steel)</t>
+  </si>
+  <si>
+    <t>pole (composite)</t>
+  </si>
+  <si>
+    <t>pole footing</t>
+  </si>
+  <si>
+    <t>pole fixtures</t>
+  </si>
+  <si>
+    <t>attachments</t>
+  </si>
+  <si>
+    <t>pole cap</t>
+  </si>
+  <si>
+    <t>steps</t>
+  </si>
+  <si>
+    <t>pole stay</t>
+  </si>
+  <si>
+    <t>pole attachment</t>
+  </si>
+  <si>
+    <t>top attachment point</t>
+  </si>
+  <si>
+    <t>thimble</t>
+  </si>
+  <si>
+    <t>wire</t>
+  </si>
+  <si>
+    <t>dead end</t>
+  </si>
+  <si>
+    <t>insulator</t>
+  </si>
+  <si>
+    <t>batten</t>
+  </si>
+  <si>
+    <t>sight guard</t>
+  </si>
+  <si>
+    <t>anchor rod</t>
+  </si>
+  <si>
+    <t>footing</t>
+  </si>
+  <si>
+    <t>pole modification</t>
+  </si>
+  <si>
+    <t>reinforcement</t>
+  </si>
+  <si>
+    <t>nail</t>
+  </si>
+  <si>
+    <t>strut</t>
+  </si>
+  <si>
+    <t>acroprop</t>
+  </si>
+  <si>
+    <t>pole accessories</t>
+  </si>
+  <si>
+    <t>fauna protection</t>
+  </si>
+  <si>
+    <t>stay protection</t>
+  </si>
+  <si>
+    <t>cattle guard post</t>
+  </si>
+  <si>
+    <t>Indicators</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>[pole] {broken} due to (termites)</t>
+  </si>
+  <si>
+    <t>[pole] {broken} due to (lightning)</t>
+  </si>
+  <si>
+    <t>nil</t>
+  </si>
+  <si>
+    <t>[pole] {broken} due to (impact)</t>
+  </si>
+  <si>
+    <t>[pole] {broken} due to (fire damage)</t>
+  </si>
+  <si>
+    <t>[pole] {broken} due to (fungal decay - internal)</t>
+  </si>
+  <si>
+    <t>[pole] {broken} due to (fungal decay - external)</t>
+  </si>
+  <si>
+    <t>[pole] {broken} due to (weathering)</t>
+  </si>
+  <si>
+    <t>[pole foundation] due to (unknown)</t>
+  </si>
+  <si>
+    <t>[pole cap] due to (unknown)</t>
+  </si>
+  <si>
+    <t>pole_cap_present</t>
+  </si>
+  <si>
+    <t>[pole stay] due to (unknown)</t>
+  </si>
+  <si>
+    <t>[pole stay] due to (impact)</t>
+  </si>
+  <si>
+    <t>[pole stay] due to (corrosion)</t>
+  </si>
+  <si>
+    <t>[pole stay] due to (bed log)</t>
+  </si>
+  <si>
+    <t>[pole top equipment] due to {cracking}</t>
+  </si>
+  <si>
+    <t>cracking_present</t>
+  </si>
+  <si>
+    <t>simple_safety_factor</t>
+  </si>
+  <si>
+    <t>sf</t>
+  </si>
+  <si>
+    <t>ssf</t>
+  </si>
+  <si>
+    <t>actual_safety_factor</t>
+  </si>
+  <si>
+    <t>dsf_calc</t>
+  </si>
+  <si>
+    <t>asf</t>
+  </si>
+  <si>
+    <t>Footing</t>
+  </si>
+  <si>
+    <t>Stay</t>
+  </si>
+  <si>
+    <t>Pole cap</t>
+  </si>
+  <si>
+    <t>top_of_pole_stregnth</t>
+  </si>
+  <si>
+    <t>Trigger</t>
+  </si>
+  <si>
+    <t>impact</t>
+  </si>
+  <si>
+    <t>tasks</t>
+  </si>
+  <si>
+    <t>task_name</t>
+  </si>
+  <si>
+    <t>Level of Failure</t>
+  </si>
+  <si>
+    <t>condition_name</t>
+  </si>
+  <si>
+    <t>termite</t>
+  </si>
+  <si>
     <t>level_3_inspection</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>max</t>
-  </si>
-  <si>
-    <t>ssf_calc</t>
-  </si>
-  <si>
-    <t>lean_angle</t>
-  </si>
-  <si>
-    <t>termite_powder</t>
-  </si>
-  <si>
-    <t>repair</t>
-  </si>
-  <si>
-    <t>ConditionTask</t>
-  </si>
-  <si>
-    <t>grp</t>
-  </si>
-  <si>
-    <t>all</t>
-  </si>
-  <si>
-    <t>reduction_factor</t>
-  </si>
-  <si>
-    <t>CAT3/4 replacement</t>
-  </si>
-  <si>
-    <t>replace</t>
-  </si>
-  <si>
-    <t>as_good_as_new</t>
-  </si>
-  <si>
-    <t>emergency replacement</t>
-  </si>
-  <si>
-    <t>fungal decay _ internal</t>
-  </si>
-  <si>
-    <t>CAT1/2 replacement</t>
-  </si>
-  <si>
-    <t>lightning</t>
-  </si>
-  <si>
-    <t>step</t>
-  </si>
-  <si>
-    <t>protection_inspection</t>
-  </si>
-  <si>
-    <t>assisted_failures</t>
-  </si>
-  <si>
-    <t>leaning</t>
-  </si>
-  <si>
-    <t>System</t>
-  </si>
-  <si>
-    <t>Sub System</t>
-  </si>
-  <si>
-    <t>Module</t>
-  </si>
-  <si>
-    <t>Maintainable Item</t>
-  </si>
-  <si>
-    <t>Component</t>
-  </si>
-  <si>
-    <t>Material</t>
-  </si>
-  <si>
-    <t>Treatment</t>
-  </si>
-  <si>
-    <t>Pole</t>
-  </si>
-  <si>
-    <t>Pole Stay</t>
-  </si>
-  <si>
-    <t>Pole Cap</t>
-  </si>
-  <si>
-    <t>Pole Footing</t>
-  </si>
-  <si>
-    <t>pole (common)</t>
-  </si>
-  <si>
-    <t>pole (timber)</t>
-  </si>
-  <si>
-    <t>pole (concrete)</t>
-  </si>
-  <si>
-    <t>pole (steel)</t>
-  </si>
-  <si>
-    <t>pole (composite)</t>
-  </si>
-  <si>
-    <t>pole footing</t>
-  </si>
-  <si>
-    <t>pole fixtures</t>
-  </si>
-  <si>
-    <t>attachments</t>
-  </si>
-  <si>
-    <t>pole cap</t>
-  </si>
-  <si>
-    <t>steps</t>
-  </si>
-  <si>
-    <t>pole stay</t>
-  </si>
-  <si>
-    <t>pole attachment</t>
-  </si>
-  <si>
-    <t>top attachment point</t>
-  </si>
-  <si>
-    <t>thimble</t>
-  </si>
-  <si>
-    <t>wire</t>
-  </si>
-  <si>
-    <t>dead end</t>
-  </si>
-  <si>
-    <t>insulator</t>
-  </si>
-  <si>
-    <t>batten</t>
-  </si>
-  <si>
-    <t>sight guard</t>
-  </si>
-  <si>
-    <t>anchor rod</t>
-  </si>
-  <si>
-    <t>footing</t>
-  </si>
-  <si>
-    <t>pole modification</t>
-  </si>
-  <si>
-    <t>reinforcement</t>
-  </si>
-  <si>
-    <t>nail</t>
-  </si>
-  <si>
-    <t>strut</t>
-  </si>
-  <si>
-    <t>acroprop</t>
-  </si>
-  <si>
-    <t>pole accessories</t>
-  </si>
-  <si>
-    <t>fauna protection</t>
-  </si>
-  <si>
-    <t>stay protection</t>
-  </si>
-  <si>
-    <t>cattle guard post</t>
-  </si>
-  <si>
-    <t>Indicators</t>
-  </si>
-  <si>
-    <t>Condition</t>
-  </si>
-  <si>
-    <t>[pole] {broken} due to (termites)</t>
-  </si>
-  <si>
-    <t>[pole] {broken} due to (lightning)</t>
-  </si>
-  <si>
-    <t>nil</t>
-  </si>
-  <si>
-    <t>[pole] {broken} due to (impact)</t>
-  </si>
-  <si>
-    <t>[pole] {broken} due to (fire damage)</t>
-  </si>
-  <si>
-    <t>[pole] {broken} due to (fungal decay - internal)</t>
-  </si>
-  <si>
-    <t>[pole] {broken} due to (fungal decay - external)</t>
-  </si>
-  <si>
-    <t>[pole] {broken} due to (weathering)</t>
-  </si>
-  <si>
-    <t>[pole foundation] due to (unknown)</t>
-  </si>
-  <si>
-    <t>[pole cap] due to (unknown)</t>
-  </si>
-  <si>
-    <t>pole_cap_present</t>
-  </si>
-  <si>
-    <t>[pole stay] due to (unknown)</t>
-  </si>
-  <si>
-    <t>[pole stay] due to (impact)</t>
-  </si>
-  <si>
-    <t>[pole stay] due to (corrosion)</t>
-  </si>
-  <si>
-    <t>[pole stay] due to (bed log)</t>
-  </si>
-  <si>
-    <t>[pole top equipment] due to {cracking}</t>
-  </si>
-  <si>
-    <t>cracking_present</t>
-  </si>
-  <si>
-    <t>simple_safety_factor</t>
-  </si>
-  <si>
-    <t>sf</t>
-  </si>
-  <si>
-    <t>ssf</t>
-  </si>
-  <si>
-    <t>actual_safety_factor</t>
-  </si>
-  <si>
-    <t>dsf_calc</t>
-  </si>
-  <si>
-    <t>asf</t>
-  </si>
-  <si>
-    <t>Footing</t>
-  </si>
-  <si>
-    <t>Stay</t>
-  </si>
-  <si>
-    <t>Pole cap</t>
-  </si>
-  <si>
-    <t>top_of_pole_stregnth</t>
-  </si>
-  <si>
-    <t>Trigger</t>
-  </si>
-  <si>
-    <t>impact</t>
-  </si>
-  <si>
-    <t>tasks</t>
-  </si>
-  <si>
-    <t>task_name</t>
-  </si>
-  <si>
-    <t>Level of Failure</t>
-  </si>
-  <si>
-    <t>condition_name</t>
-  </si>
-  <si>
-    <t>termite</t>
   </si>
   <si>
     <t>any</t>
@@ -2278,36 +2281,36 @@
   <sheetData>
     <row r="3" spans="1:19">
       <c r="A3" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F5" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="N6" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -2315,52 +2318,52 @@
         <v>176</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="13" spans="1:19">
       <c r="F13" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="O13" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="Q13" t="s">
         <v>151</v>
       </c>
       <c r="S13" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:19">
       <c r="F14" s="12" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="O14" t="s">
         <v>148</v>
       </c>
       <c r="Q14" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="S14" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" spans="1:19">
       <c r="F15" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J15" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="O15" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="Q15" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="S15" t="s">
         <v>110</v>
@@ -2368,44 +2371,44 @@
     </row>
     <row r="16" spans="1:19">
       <c r="F16" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="Q16" t="s">
         <v>97</v>
       </c>
       <c r="S16" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="17" spans="1:19">
       <c r="F17" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="O17" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="Q17" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="18" spans="1:19">
       <c r="O18" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20" spans="1:19">
       <c r="F20" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="27" spans="1:19">
       <c r="A27" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="31" spans="1:19">
       <c r="D31" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E31" t="s">
         <v>6</v>
@@ -2417,7 +2420,7 @@
         <v>90</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="P31" s="1" t="s">
         <v>96</v>
@@ -2431,7 +2434,7 @@
     </row>
     <row r="32" spans="1:19">
       <c r="A32" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="J32" t="s">
         <v>24</v>
@@ -2451,7 +2454,7 @@
         <v>51</v>
       </c>
       <c r="R33" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="S33">
         <v>0</v>
@@ -2459,13 +2462,13 @@
     </row>
     <row r="34" spans="2:19">
       <c r="C34" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="K34" t="s">
         <v>54</v>
       </c>
       <c r="R34" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="S34">
         <v>0.5</v>
@@ -2473,16 +2476,16 @@
     </row>
     <row r="35" spans="2:19">
       <c r="C35" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D35" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="G35" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="L35" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="R35" t="s">
         <v>97</v>
@@ -2493,13 +2496,13 @@
     </row>
     <row r="36" spans="2:19">
       <c r="D36" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="L36" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="R36" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="S36">
         <v>1</v>
@@ -2515,7 +2518,7 @@
     </row>
     <row r="38" spans="2:19">
       <c r="C38" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E38" t="s">
         <v>148</v>
@@ -2526,10 +2529,10 @@
     </row>
     <row r="39" spans="2:19">
       <c r="C39" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E39" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="J39" t="s">
         <v>177</v>
@@ -2552,12 +2555,12 @@
     </row>
     <row r="52" spans="1:12">
       <c r="H52" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>111</v>
@@ -2569,12 +2572,12 @@
         <v>148</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="54" spans="1:12">
       <c r="E54" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="F54">
         <v>4</v>
@@ -2608,17 +2611,17 @@
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="59" spans="1:12">
       <c r="F59" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="60" spans="1:12">
       <c r="B60" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E60" t="s">
         <v>96</v>
@@ -2626,12 +2629,12 @@
     </row>
     <row r="61" spans="1:12">
       <c r="E61" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="62" spans="1:12">
       <c r="E62" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -2639,45 +2642,45 @@
         <v>177</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="B68" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B69">
         <v>4</v>
       </c>
       <c r="C69" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B70">
         <v>250</v>
       </c>
       <c r="C70" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B71">
         <v>12.5</v>
       </c>
       <c r="C71" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -2709,48 +2712,48 @@
   <sheetData>
     <row r="2" spans="1:19">
       <c r="A2" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:19">
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="B4" t="s">
+        <v>305</v>
+      </c>
+      <c r="I4" t="s">
+        <v>303</v>
+      </c>
+      <c r="J4" t="s">
         <v>304</v>
       </c>
-      <c r="I4" t="s">
-        <v>302</v>
-      </c>
-      <c r="J4" t="s">
-        <v>303</v>
-      </c>
       <c r="P4" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="R4" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="S4" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="B5" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="H5" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="I5" s="3">
         <v>14</v>
@@ -2760,18 +2763,18 @@
       </c>
       <c r="P5" s="1"/>
       <c r="Q5" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="R5" s="41" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="S5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="6" spans="1:19">
       <c r="H6" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="I6">
         <f>I5/4</f>
@@ -2783,51 +2786,51 @@
       </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="R6" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="S6" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="P7" s="1"/>
       <c r="Q7" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="R7" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="S7" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="8" spans="1:19">
       <c r="H8" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="I8" s="5">
         <v>320</v>
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="R8" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="S8" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="H9" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="I9" s="5">
         <v>100</v>
@@ -2835,7 +2838,7 @@
     </row>
     <row r="10" spans="1:19">
       <c r="H10" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="I10" s="5">
         <v>10</v>
@@ -2843,12 +2846,12 @@
     </row>
     <row r="11" spans="1:19">
       <c r="B11" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="12" spans="1:19">
       <c r="B12" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="I12" s="9">
         <v>3.7</v>
@@ -2860,20 +2863,20 @@
     </row>
     <row r="16" spans="1:19">
       <c r="J16" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="M16" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="19" spans="10:10">
       <c r="J19" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="1048576" spans="15:15">
       <c r="O1048576" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -3152,8 +3155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA0734F-FFBE-4DAF-BDE5-A12359370A0D}">
   <dimension ref="A1:AX35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AE37" sqref="AE37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1"/>
@@ -5292,7 +5295,7 @@
         <v>5</v>
       </c>
       <c r="AE31" s="91" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="AF31" s="15" t="s">
         <v>84</v>
@@ -6670,7 +6673,7 @@
         <v>151</v>
       </c>
       <c r="M4" s="15" t="s">
-        <v>83</v>
+        <v>183</v>
       </c>
       <c r="N4" s="15" t="s">
         <v>84</v>
@@ -6685,10 +6688,10 @@
         <v>1</v>
       </c>
       <c r="R4" s="18" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="S4" s="18" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="T4" s="18"/>
       <c r="U4" s="18"/>
@@ -6748,7 +6751,7 @@
         <v>92</v>
       </c>
       <c r="L6" s="15" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="Q6" s="16" t="b">
         <v>1</v>
@@ -6836,7 +6839,7 @@
     </row>
     <row r="9" spans="1:35" s="15" customFormat="1">
       <c r="C9" s="15" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E9" s="15">
         <v>1</v>
@@ -6983,7 +6986,7 @@
         <v>28</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>80</v>
@@ -6995,7 +6998,7 @@
         <v>50</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H15" s="15" t="s">
         <v>80</v>
@@ -7007,7 +7010,7 @@
         <v>5</v>
       </c>
       <c r="M15" s="15" t="s">
-        <v>83</v>
+        <v>183</v>
       </c>
       <c r="N15" s="15" t="s">
         <v>84</v>
@@ -7022,10 +7025,10 @@
         <v>1</v>
       </c>
       <c r="R15" s="18" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="S15" s="18" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="T15" s="18"/>
       <c r="U15" s="18"/>
@@ -7066,7 +7069,7 @@
     </row>
     <row r="16" spans="1:35" s="15" customFormat="1">
       <c r="C16" s="15" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E16" s="15">
         <v>0.9</v>
@@ -7157,7 +7160,7 @@
     </row>
     <row r="18" spans="1:35" s="15" customFormat="1">
       <c r="C18" s="15" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E18" s="15">
         <v>1</v>
@@ -7269,7 +7272,7 @@
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21" s="15" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E21" s="15">
         <v>1</v>
@@ -7284,10 +7287,10 @@
         <v>96</v>
       </c>
       <c r="Q21" s="15" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="R21" s="15" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="S21" s="15" t="b">
         <v>1</v>
@@ -7349,7 +7352,7 @@
         <v>2</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="L23" s="15" t="s">
         <v>6</v>
@@ -7407,7 +7410,7 @@
         <v>50</v>
       </c>
       <c r="AG23" s="16" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="AI23" s="47"/>
     </row>
@@ -7445,7 +7448,7 @@
         <v>50</v>
       </c>
       <c r="AG24" s="16" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="AI24" s="47"/>
     </row>
@@ -7593,16 +7596,16 @@
         <v>110</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>59</v>
@@ -7625,7 +7628,7 @@
         <v>80</v>
       </c>
       <c r="D3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E3" t="s">
         <v>86</v>
@@ -7639,7 +7642,7 @@
         <v>89</v>
       </c>
       <c r="D4" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E4" t="s">
         <v>86</v>
@@ -7647,7 +7650,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="C5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -7659,7 +7662,7 @@
         <v>100000</v>
       </c>
       <c r="G5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -7712,16 +7715,16 @@
         <v>110</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>59</v>
@@ -7738,7 +7741,7 @@
         <v>80</v>
       </c>
       <c r="D13" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E13" t="s">
         <v>86</v>
@@ -7747,7 +7750,7 @@
         <v>50</v>
       </c>
       <c r="H13" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -7755,7 +7758,7 @@
         <v>89</v>
       </c>
       <c r="D14" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E14" t="s">
         <v>86</v>
@@ -7834,226 +7837,226 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="32" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C4" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="32" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C5" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="32" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C6" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="32" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C7" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="32" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C8" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="32" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C9" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="32" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C10" s="34" t="e">
         <v>#REF!</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="32" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C11" s="34" t="e">
         <v>#REF!</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="32" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C12" s="34" t="e">
         <v>#REF!</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="32" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C13" s="34" t="e">
         <v>#REF!</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="32" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C14" s="34" t="e">
         <v>#REF!</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="32" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C15" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="32" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C16" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="33" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C17" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="33" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C18" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="32" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C19" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -8074,72 +8077,72 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="32" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C22" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="33" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B23" s="33" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C23" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D23" s="33" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="32" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B24" s="32" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C24" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D24" s="32" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="33" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B25" s="33" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C25" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D25" s="33" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="32" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C26" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D26" s="32" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -8152,86 +8155,86 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="32" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C28" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D28" s="32" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="33" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C29" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D29" s="33" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="32" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C30" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D30" s="32" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="33" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B31" s="33" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C31" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D31" s="33" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="32" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C32" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D32" s="32" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="33" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C33" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D33" s="36" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -8244,72 +8247,72 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="33" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B35" s="33" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C35" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D35" s="33" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="32" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B36" s="32" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C36" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D36" s="32" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="33" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B37" s="33" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C37" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D37" s="33" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="32" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B38" s="32" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C38" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D38" s="32" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="33" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B39" s="33" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C39" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D39" s="33" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -8330,16 +8333,16 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="32" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B42" s="32" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C42" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D42" s="32" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -8352,226 +8355,226 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="32" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B44" s="39" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C44" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D44" s="32" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="33" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B45" s="36" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C45" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D45" s="33" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="32" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B46" s="39" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C46" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D46" s="32" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="33" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B47" s="36" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C47" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D47" s="33" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="32" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B48" s="39" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C48" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D48" s="32" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="33" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B49" s="36" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C49" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D49" s="33" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="32" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B50" s="39" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C50" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D50" s="32" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="33" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B51" s="36" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C51" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D51" s="33" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="32" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B52" s="39" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C52" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D52" s="32" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="33" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B53" s="33" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C53" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D53" s="33" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="32" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B54" s="32" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C54" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D54" s="32" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="33" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B55" s="33" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C55" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D55" s="33" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="32" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B56" s="32" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C56" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D56" s="32" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="33" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B57" s="33" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C57" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D57" s="33" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="32" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B58" s="39" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C58" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D58" s="32" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="33" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B59" s="36" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C59" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D59" s="33" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -8584,86 +8587,86 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="33" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B61" s="36" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C61" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D61" s="33" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="32" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B62" s="39" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C62" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D62" s="32" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="33" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B63" s="33" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C63" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D63" s="33" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="32" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B64" s="32" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C64" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D64" s="32" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="33" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B65" s="33" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C65" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D65" s="33" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="32" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B66" s="32" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C66" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D66" s="32" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -8684,44 +8687,44 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="33" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B69" s="33" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C69" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D69" s="33" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="32" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B70" s="32" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C70" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D70" s="32" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="33" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B71" s="33" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C71" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D71" s="33" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
before looking for timeline error
</commit_message>
<xml_diff>
--- a/data/inputs/Asset Model - Pole - Demo.xlsx
+++ b/data/inputs/Asset Model - Pole - Demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtreseder\OneDrive - KPMG\Documents\3. Client\Essential Energy\Probability of Failure Model\pof\data\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2084" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FCB75139-2875-4347-A496-BF1D5E822264}"/>
+  <xr:revisionPtr revIDLastSave="2085" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DFE9973C-736B-4B16-A23F-93AC5197215F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="320">
   <si>
     <t>Cause</t>
   </si>
@@ -404,13 +404,10 @@
     <t>as_good_as_new</t>
   </si>
   <si>
-    <t>emergency replacement</t>
+    <t>CAT1/2 replacement</t>
   </si>
   <si>
     <t>fungal decay _ internal</t>
-  </si>
-  <si>
-    <t>CAT1/2 replacement</t>
   </si>
   <si>
     <t>lightning</t>
@@ -2281,134 +2278,134 @@
   <sheetData>
     <row r="3" spans="1:19">
       <c r="A3" t="s">
+        <v>251</v>
+      </c>
+      <c r="F3" t="s">
         <v>252</v>
-      </c>
-      <c r="F3" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" t="s">
+        <v>253</v>
+      </c>
+      <c r="F5" t="s">
         <v>254</v>
-      </c>
-      <c r="F5" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
+        <v>255</v>
+      </c>
+      <c r="N6" t="s">
         <v>256</v>
-      </c>
-      <c r="N6" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" spans="1:19">
       <c r="O12" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q12" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="S12" s="1" t="s">
         <v>260</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="13" spans="1:19">
       <c r="F13" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="O13" t="s">
         <v>262</v>
       </c>
-      <c r="O13" t="s">
+      <c r="Q13" t="s">
+        <v>150</v>
+      </c>
+      <c r="S13" t="s">
         <v>263</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>151</v>
-      </c>
-      <c r="S13" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:19">
       <c r="F14" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="O14" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q14" t="s">
         <v>265</v>
       </c>
-      <c r="O14" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q14" t="s">
+      <c r="S14" t="s">
         <v>266</v>
-      </c>
-      <c r="S14" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="15" spans="1:19">
       <c r="F15" t="s">
+        <v>267</v>
+      </c>
+      <c r="J15" t="s">
         <v>268</v>
       </c>
-      <c r="J15" t="s">
+      <c r="O15" t="s">
         <v>269</v>
       </c>
-      <c r="O15" t="s">
+      <c r="Q15" t="s">
         <v>270</v>
       </c>
-      <c r="Q15" t="s">
-        <v>271</v>
-      </c>
       <c r="S15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:19">
       <c r="F16" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="Q16" t="s">
         <v>97</v>
       </c>
       <c r="S16" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="17" spans="1:19">
       <c r="F17" t="s">
+        <v>273</v>
+      </c>
+      <c r="O17" t="s">
         <v>274</v>
       </c>
-      <c r="O17" t="s">
+      <c r="Q17" t="s">
         <v>275</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="18" spans="1:19">
       <c r="O18" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="20" spans="1:19">
       <c r="F20" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="27" spans="1:19">
       <c r="A27" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="31" spans="1:19">
       <c r="D31" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E31" t="s">
         <v>6</v>
@@ -2420,13 +2417,13 @@
         <v>90</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P31" s="1" t="s">
         <v>96</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="S31" s="1" t="s">
         <v>94</v>
@@ -2434,27 +2431,27 @@
     </row>
     <row r="32" spans="1:19">
       <c r="A32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J32" t="s">
         <v>24</v>
       </c>
       <c r="R32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="S32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="2:19">
       <c r="B33" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K33" t="s">
         <v>51</v>
       </c>
       <c r="R33" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="S33">
         <v>0</v>
@@ -2462,13 +2459,13 @@
     </row>
     <row r="34" spans="2:19">
       <c r="C34" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K34" t="s">
         <v>54</v>
       </c>
       <c r="R34" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="S34">
         <v>0.5</v>
@@ -2476,16 +2473,16 @@
     </row>
     <row r="35" spans="2:19">
       <c r="C35" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D35" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G35" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="L35" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R35" t="s">
         <v>97</v>
@@ -2496,13 +2493,13 @@
     </row>
     <row r="36" spans="2:19">
       <c r="D36" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L36" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="R36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="S36">
         <v>1</v>
@@ -2518,10 +2515,10 @@
     </row>
     <row r="38" spans="2:19">
       <c r="C38" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K38" t="s">
         <v>2</v>
@@ -2529,13 +2526,13 @@
     </row>
     <row r="39" spans="2:19">
       <c r="C39" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E39" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J39" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="40" spans="2:19">
@@ -2555,29 +2552,29 @@
     </row>
     <row r="52" spans="1:12">
       <c r="H52" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="I53" s="1" t="s">
         <v>286</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="54" spans="1:12">
       <c r="E54" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F54">
         <v>4</v>
@@ -2611,17 +2608,17 @@
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="59" spans="1:12">
       <c r="F59" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="60" spans="1:12">
       <c r="B60" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E60" t="s">
         <v>96</v>
@@ -2629,58 +2626,58 @@
     </row>
     <row r="61" spans="1:12">
       <c r="E61" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="62" spans="1:12">
       <c r="E62" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="B65" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="B68" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B69">
         <v>4</v>
       </c>
       <c r="C69" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B70">
         <v>250</v>
       </c>
       <c r="C70" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B71">
         <v>12.5</v>
       </c>
       <c r="C71" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -2712,48 +2709,48 @@
   <sheetData>
     <row r="2" spans="1:19">
       <c r="A2" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:19">
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>303</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="B4" t="s">
+        <v>304</v>
+      </c>
+      <c r="I4" t="s">
+        <v>302</v>
+      </c>
+      <c r="J4" t="s">
+        <v>303</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="I4" t="s">
-        <v>303</v>
-      </c>
-      <c r="J4" t="s">
-        <v>304</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" t="s">
         <v>306</v>
       </c>
-      <c r="R4" t="s">
-        <v>307</v>
-      </c>
       <c r="S4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="B5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I5" s="3">
         <v>14</v>
@@ -2763,18 +2760,18 @@
       </c>
       <c r="P5" s="1"/>
       <c r="Q5" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="R5" s="41" t="s">
         <v>309</v>
       </c>
-      <c r="R5" s="41" t="s">
+      <c r="S5" t="s">
         <v>310</v>
-      </c>
-      <c r="S5" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="6" spans="1:19">
       <c r="H6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I6">
         <f>I5/4</f>
@@ -2786,51 +2783,51 @@
       </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="R6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="S6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="P7" s="1"/>
       <c r="Q7" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="R7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="S7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="8" spans="1:19">
       <c r="H8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I8" s="5">
         <v>320</v>
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="R8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="S8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="I9" s="5">
         <v>100</v>
@@ -2838,7 +2835,7 @@
     </row>
     <row r="10" spans="1:19">
       <c r="H10" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I10" s="5">
         <v>10</v>
@@ -2846,12 +2843,12 @@
     </row>
     <row r="11" spans="1:19">
       <c r="B11" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="12" spans="1:19">
       <c r="B12" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I12" s="9">
         <v>3.7</v>
@@ -2863,20 +2860,20 @@
     </row>
     <row r="16" spans="1:19">
       <c r="J16" t="s">
+        <v>317</v>
+      </c>
+      <c r="M16" t="s">
         <v>318</v>
-      </c>
-      <c r="M16" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="19" spans="10:10">
       <c r="J19" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="1048576" spans="15:15">
       <c r="O1048576" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -3155,8 +3152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA0734F-FFBE-4DAF-BDE5-A12359370A0D}">
   <dimension ref="A1:AX35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AE37" sqref="AE37"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1"/>
@@ -4723,7 +4720,7 @@
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
       <c r="U23" s="15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="V23" s="15"/>
       <c r="W23" s="15">
@@ -4847,13 +4844,13 @@
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
       <c r="I25" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J25" s="15">
         <v>1</v>
       </c>
       <c r="K25" s="41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L25" s="41">
         <v>0</v>
@@ -4875,7 +4872,7 @@
       <c r="S25" s="41"/>
       <c r="T25" s="93"/>
       <c r="U25" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="V25" s="15"/>
       <c r="W25" s="15">
@@ -4903,7 +4900,7 @@
         <v>1</v>
       </c>
       <c r="AE25" s="91" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AF25" s="15"/>
       <c r="AG25" s="15"/>
@@ -5117,7 +5114,7 @@
       <c r="A29" s="15"/>
       <c r="B29" s="15"/>
       <c r="U29" s="15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="V29" s="15"/>
       <c r="W29" s="15">
@@ -5241,7 +5238,7 @@
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
       <c r="I31" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J31" s="15">
         <v>0</v>
@@ -5295,7 +5292,7 @@
         <v>5</v>
       </c>
       <c r="AE31" s="91" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AF31" s="15" t="s">
         <v>84</v>
@@ -5401,7 +5398,7 @@
       <c r="S33" s="15"/>
       <c r="T33" s="91"/>
       <c r="U33" s="15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="V33" s="15"/>
       <c r="W33" s="15">
@@ -5699,39 +5696,39 @@
     <row r="2" spans="1:20">
       <c r="J2" s="1"/>
       <c r="Q2" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="R2" s="27" t="s">
+      <c r="S2" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="S2" s="27" t="s">
+      <c r="T2" s="27" t="s">
         <v>108</v>
-      </c>
-      <c r="T2" s="27" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" t="s">
         <v>110</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>111</v>
-      </c>
-      <c r="D3" t="s">
-        <v>112</v>
       </c>
       <c r="Q3" s="28"/>
     </row>
     <row r="4" spans="1:20">
       <c r="B4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q4" s="29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="R4" s="29"/>
       <c r="S4" s="29"/>
@@ -5739,7 +5736,7 @@
     </row>
     <row r="5" spans="1:20">
       <c r="B5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Q5" s="29"/>
       <c r="R5" s="30" t="s">
@@ -5750,7 +5747,7 @@
     </row>
     <row r="6" spans="1:20">
       <c r="B6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Q6" s="31"/>
       <c r="R6" s="31"/>
@@ -5761,72 +5758,72 @@
     </row>
     <row r="7" spans="1:20">
       <c r="B7" t="s">
+        <v>115</v>
+      </c>
+      <c r="T7" t="s">
         <v>116</v>
-      </c>
-      <c r="T7" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="T8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="T9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="T10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="T11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="Q12" s="31"/>
       <c r="R12" s="31"/>
       <c r="S12" s="31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="T12" s="31"/>
     </row>
     <row r="13" spans="1:20">
       <c r="T13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="Q14" s="31"/>
       <c r="R14" s="31"/>
       <c r="S14" s="31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="T14" s="31"/>
     </row>
     <row r="15" spans="1:20">
       <c r="T15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:20">
       <c r="T16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="17:20">
       <c r="T17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="17:20">
       <c r="Q18" s="29"/>
       <c r="R18" s="30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="S18" s="29"/>
       <c r="T18" s="29"/>
@@ -5835,85 +5832,85 @@
       <c r="Q19" s="31"/>
       <c r="R19" s="31"/>
       <c r="S19" s="31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="T19" s="31"/>
     </row>
     <row r="20" spans="17:20">
       <c r="T20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="17:20">
       <c r="Q21" s="28"/>
       <c r="S21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="17:20">
       <c r="Q22" s="28"/>
       <c r="T22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="17:20">
       <c r="Q23" s="28"/>
       <c r="S23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="17:20">
       <c r="Q24" s="28"/>
       <c r="T24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="17:20">
       <c r="Q25" s="28"/>
       <c r="T25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="17:20">
       <c r="Q26" s="28"/>
       <c r="S26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="17:20">
       <c r="Q27" s="28"/>
       <c r="S27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="17:20">
       <c r="Q28" s="28"/>
       <c r="T28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="29" spans="17:20">
       <c r="Q29" s="28"/>
       <c r="S29" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="17:20">
       <c r="Q30" s="28"/>
       <c r="T30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="17:20">
       <c r="Q31" s="28"/>
       <c r="T31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="17:20">
       <c r="Q32" s="29"/>
       <c r="R32" s="30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S32" s="29"/>
       <c r="T32" s="29"/>
@@ -5922,34 +5919,34 @@
       <c r="Q33" s="31"/>
       <c r="R33" s="31"/>
       <c r="S33" s="31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="T33" s="31"/>
     </row>
     <row r="34" spans="17:20">
       <c r="Q34" s="28"/>
       <c r="T34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="17:20">
       <c r="Q35" s="31"/>
       <c r="R35" s="31"/>
       <c r="S35" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T35" s="31"/>
     </row>
     <row r="36" spans="17:20">
       <c r="Q36" s="28"/>
       <c r="T36" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="37" spans="17:20">
       <c r="Q37" s="29"/>
       <c r="R37" s="30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="S37" s="29"/>
       <c r="T37" s="29"/>
@@ -5958,28 +5955,28 @@
       <c r="Q38" s="31"/>
       <c r="R38" s="31"/>
       <c r="S38" s="31" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="T38" s="31"/>
     </row>
     <row r="39" spans="17:20">
       <c r="Q39" s="28"/>
       <c r="T39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="40" spans="17:20">
       <c r="Q40" s="31"/>
       <c r="R40" s="31"/>
       <c r="S40" s="31" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T40" s="31"/>
     </row>
     <row r="41" spans="17:20">
       <c r="Q41" s="28"/>
       <c r="T41" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -6020,7 +6017,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
       <c r="H1" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -6046,12 +6043,12 @@
         <v>15</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B3">
         <v>50</v>
@@ -6091,10 +6088,10 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -6103,12 +6100,12 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B6">
         <v>50</v>
@@ -6120,18 +6117,18 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H7" t="s">
         <v>38</v>
@@ -6139,7 +6136,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B8">
         <v>80</v>
@@ -6165,7 +6162,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E9" t="s">
         <v>79</v>
@@ -6176,7 +6173,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E10" t="s">
         <v>79</v>
@@ -6187,7 +6184,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B11" s="42"/>
       <c r="C11" s="42"/>
@@ -6195,7 +6192,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B12">
         <v>1000</v>
@@ -6216,13 +6213,13 @@
         <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J12" s="45"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F13">
         <v>25</v>
@@ -6230,22 +6227,22 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B19">
         <v>50</v>
@@ -6257,15 +6254,15 @@
         <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B20">
         <v>50</v>
@@ -6277,10 +6274,10 @@
         <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -6306,10 +6303,10 @@
   <sheetData>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>16</v>
@@ -6323,7 +6320,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -6348,10 +6345,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="B5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C5" t="s">
         <v>166</v>
-      </c>
-      <c r="C5" t="s">
-        <v>167</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -6360,53 +6357,53 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="B6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C6" t="s">
         <v>169</v>
-      </c>
-      <c r="C6" t="s">
-        <v>170</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="B10" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3">
@@ -6469,7 +6466,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="R1" s="22"/>
       <c r="S1" s="22"/>
@@ -6481,7 +6478,7 @@
       <c r="Y1" s="24"/>
       <c r="Z1" s="52"/>
       <c r="AA1" s="21" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AB1" s="21"/>
       <c r="AC1" s="21"/>
@@ -6494,7 +6491,7 @@
     </row>
     <row r="2" spans="1:35" s="1" customFormat="1">
       <c r="C2" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E2" s="25"/>
       <c r="F2" s="25"/>
@@ -6535,7 +6532,7 @@
       <c r="AC2" s="21"/>
       <c r="AD2" s="49"/>
       <c r="AE2" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AF2" s="4"/>
       <c r="AG2" s="4"/>
@@ -6550,7 +6547,7 @@
         <v>48</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E3" s="25" t="s">
         <v>58</v>
@@ -6574,7 +6571,7 @@
         <v>63</v>
       </c>
       <c r="L3" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>64</v>
@@ -6605,7 +6602,7 @@
       </c>
       <c r="V3" s="55"/>
       <c r="W3" s="23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="X3" s="24" t="s">
         <v>26</v>
@@ -6625,7 +6622,7 @@
       </c>
       <c r="AD3" s="49"/>
       <c r="AE3" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AF3" s="4" t="s">
         <v>75</v>
@@ -6643,7 +6640,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>80</v>
@@ -6670,10 +6667,10 @@
         <v>5</v>
       </c>
       <c r="L4" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M4" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N4" s="15" t="s">
         <v>84</v>
@@ -6688,10 +6685,10 @@
         <v>1</v>
       </c>
       <c r="R4" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="S4" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="T4" s="18"/>
       <c r="U4" s="18"/>
@@ -6751,7 +6748,7 @@
         <v>92</v>
       </c>
       <c r="L6" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="Q6" s="16" t="b">
         <v>1</v>
@@ -6839,7 +6836,7 @@
     </row>
     <row r="9" spans="1:35" s="15" customFormat="1">
       <c r="C9" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E9" s="15">
         <v>1</v>
@@ -6986,7 +6983,7 @@
         <v>28</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>80</v>
@@ -6998,7 +6995,7 @@
         <v>50</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H15" s="15" t="s">
         <v>80</v>
@@ -7010,7 +7007,7 @@
         <v>5</v>
       </c>
       <c r="M15" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N15" s="15" t="s">
         <v>84</v>
@@ -7025,51 +7022,51 @@
         <v>1</v>
       </c>
       <c r="R15" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="S15" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="T15" s="18"/>
       <c r="U15" s="18"/>
       <c r="V15" s="50"/>
       <c r="W15" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X15" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Y15" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Z15" s="50"/>
       <c r="AA15" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AB15" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AC15" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AD15" s="50"/>
       <c r="AE15" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AF15" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AG15" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AH15" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AI15" s="47"/>
     </row>
     <row r="16" spans="1:35" s="15" customFormat="1">
       <c r="C16" s="15" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E16" s="15">
         <v>0.9</v>
@@ -7116,16 +7113,16 @@
       </c>
       <c r="AD16" s="50"/>
       <c r="AE16" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AF16" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AG16" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AH16" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AI16" s="47"/>
     </row>
@@ -7160,7 +7157,7 @@
     </row>
     <row r="18" spans="1:35" s="15" customFormat="1">
       <c r="C18" s="15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E18" s="15">
         <v>1</v>
@@ -7272,7 +7269,7 @@
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E21" s="15">
         <v>1</v>
@@ -7287,33 +7284,33 @@
         <v>96</v>
       </c>
       <c r="Q21" s="15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="R21" s="15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="S21" s="15" t="b">
         <v>1</v>
       </c>
       <c r="V21" s="47"/>
       <c r="W21" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X21" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Y21" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Z21" s="47"/>
       <c r="AA21" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AB21" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AC21" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AD21" s="47"/>
       <c r="AE21"/>
@@ -7340,7 +7337,7 @@
     </row>
     <row r="23" spans="1:35" s="15" customFormat="1">
       <c r="C23" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E23" s="15">
         <v>0.9</v>
@@ -7352,13 +7349,13 @@
         <v>2</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L23" s="15" t="s">
         <v>6</v>
       </c>
       <c r="M23" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N23" s="15" t="s">
         <v>85</v>
@@ -7394,13 +7391,13 @@
       </c>
       <c r="Z23" s="53"/>
       <c r="AA23" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AB23" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AC23" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AD23" s="50"/>
       <c r="AE23" s="16" t="s">
@@ -7410,7 +7407,7 @@
         <v>50</v>
       </c>
       <c r="AG23" s="16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AI23" s="47"/>
     </row>
@@ -7432,13 +7429,13 @@
       </c>
       <c r="Z24" s="53"/>
       <c r="AA24" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AB24" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AC24" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AD24" s="50"/>
       <c r="AE24" s="16" t="s">
@@ -7448,7 +7445,7 @@
         <v>50</v>
       </c>
       <c r="AG24" s="16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AI24" s="47"/>
     </row>
@@ -7593,19 +7590,19 @@
   <sheetData>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>59</v>
@@ -7619,16 +7616,16 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C3" t="s">
         <v>80</v>
       </c>
       <c r="D3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E3" t="s">
         <v>86</v>
@@ -7642,7 +7639,7 @@
         <v>89</v>
       </c>
       <c r="D4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E4" t="s">
         <v>86</v>
@@ -7650,7 +7647,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="C5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -7662,7 +7659,7 @@
         <v>100000</v>
       </c>
       <c r="G5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -7712,19 +7709,19 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>59</v>
@@ -7732,16 +7729,16 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C13" t="s">
         <v>80</v>
       </c>
       <c r="D13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E13" t="s">
         <v>86</v>
@@ -7750,7 +7747,7 @@
         <v>50</v>
       </c>
       <c r="H13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -7758,7 +7755,7 @@
         <v>89</v>
       </c>
       <c r="D14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E14" t="s">
         <v>86</v>
@@ -7769,7 +7766,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="C15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -7837,226 +7834,226 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="B4" s="32" t="s">
         <v>201</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>202</v>
       </c>
       <c r="C4" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="B5" s="33" t="s">
         <v>201</v>
-      </c>
-      <c r="B5" s="33" t="s">
-        <v>202</v>
       </c>
       <c r="C5" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="B6" s="32" t="s">
         <v>201</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>202</v>
       </c>
       <c r="C6" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="B7" s="33" t="s">
         <v>201</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>202</v>
       </c>
       <c r="C7" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="B8" s="32" t="s">
         <v>201</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>202</v>
       </c>
       <c r="C8" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="B9" s="33" t="s">
         <v>201</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>202</v>
       </c>
       <c r="C9" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="B10" s="34" t="s">
         <v>201</v>
-      </c>
-      <c r="B10" s="34" t="s">
-        <v>202</v>
       </c>
       <c r="C10" s="34" t="e">
         <v>#REF!</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="B11" s="34" t="s">
         <v>201</v>
-      </c>
-      <c r="B11" s="34" t="s">
-        <v>202</v>
       </c>
       <c r="C11" s="34" t="e">
         <v>#REF!</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="B12" s="34" t="s">
         <v>201</v>
-      </c>
-      <c r="B12" s="34" t="s">
-        <v>202</v>
       </c>
       <c r="C12" s="34" t="e">
         <v>#REF!</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="B13" s="34" t="s">
         <v>201</v>
-      </c>
-      <c r="B13" s="34" t="s">
-        <v>202</v>
       </c>
       <c r="C13" s="34" t="e">
         <v>#REF!</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="B14" s="34" t="s">
         <v>201</v>
-      </c>
-      <c r="B14" s="34" t="s">
-        <v>202</v>
       </c>
       <c r="C14" s="34" t="e">
         <v>#REF!</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="B15" s="34" t="s">
         <v>201</v>
-      </c>
-      <c r="B15" s="34" t="s">
-        <v>202</v>
       </c>
       <c r="C15" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="32" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C16" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="33" t="s">
+        <v>215</v>
+      </c>
+      <c r="B17" s="33" t="s">
         <v>216</v>
-      </c>
-      <c r="B17" s="33" t="s">
-        <v>217</v>
       </c>
       <c r="C17" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="33" t="s">
+        <v>215</v>
+      </c>
+      <c r="B18" s="32" t="s">
         <v>216</v>
-      </c>
-      <c r="B18" s="32" t="s">
-        <v>217</v>
       </c>
       <c r="C18" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="32" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C19" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -8077,72 +8074,72 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="32" t="s">
+        <v>218</v>
+      </c>
+      <c r="B22" s="32" t="s">
         <v>219</v>
-      </c>
-      <c r="B22" s="32" t="s">
-        <v>220</v>
       </c>
       <c r="C22" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="33" t="s">
+        <v>218</v>
+      </c>
+      <c r="B23" s="33" t="s">
         <v>219</v>
-      </c>
-      <c r="B23" s="33" t="s">
-        <v>220</v>
       </c>
       <c r="C23" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D23" s="33" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="32" t="s">
+        <v>218</v>
+      </c>
+      <c r="B24" s="32" t="s">
         <v>219</v>
-      </c>
-      <c r="B24" s="32" t="s">
-        <v>220</v>
       </c>
       <c r="C24" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D24" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B25" s="33" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C25" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D25" s="33" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="32" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C26" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D26" s="32" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -8155,86 +8152,86 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="32" t="s">
+        <v>225</v>
+      </c>
+      <c r="B28" s="32" t="s">
         <v>226</v>
-      </c>
-      <c r="B28" s="32" t="s">
-        <v>227</v>
       </c>
       <c r="C28" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D28" s="32" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="33" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C29" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D29" s="33" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="32" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C30" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D30" s="32" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="33" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B31" s="33" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C31" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D31" s="33" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="32" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C32" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D32" s="32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="33" t="s">
+        <v>230</v>
+      </c>
+      <c r="B33" s="33" t="s">
         <v>231</v>
-      </c>
-      <c r="B33" s="33" t="s">
-        <v>232</v>
       </c>
       <c r="C33" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D33" s="36" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -8247,72 +8244,72 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="33" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B35" s="33" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C35" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D35" s="33" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="32" t="s">
+        <v>232</v>
+      </c>
+      <c r="B36" s="32" t="s">
         <v>233</v>
-      </c>
-      <c r="B36" s="32" t="s">
-        <v>234</v>
       </c>
       <c r="C36" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D36" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="33" t="s">
+        <v>232</v>
+      </c>
+      <c r="B37" s="33" t="s">
         <v>233</v>
-      </c>
-      <c r="B37" s="33" t="s">
-        <v>234</v>
       </c>
       <c r="C37" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D37" s="33" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="32" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B38" s="32" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C38" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D38" s="32" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="33" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B39" s="33" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C39" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D39" s="33" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -8333,16 +8330,16 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="32" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B42" s="32" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C42" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D42" s="32" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -8355,226 +8352,226 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="32" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B44" s="39" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C44" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D44" s="32" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="33" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B45" s="36" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C45" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D45" s="33" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="32" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B46" s="39" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C46" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D46" s="32" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="33" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B47" s="36" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C47" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D47" s="33" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="32" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B48" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C48" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D48" s="32" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="33" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B49" s="36" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C49" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D49" s="33" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="32" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B50" s="39" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C50" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D50" s="32" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="33" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B51" s="36" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C51" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D51" s="33" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="32" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B52" s="39" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C52" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D52" s="32" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="33" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B53" s="33" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C53" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D53" s="33" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="32" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B54" s="32" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C54" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D54" s="32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="33" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B55" s="33" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C55" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D55" s="33" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="32" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B56" s="32" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C56" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D56" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="33" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B57" s="33" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C57" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D57" s="33" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="32" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B58" s="39" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C58" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D58" s="32" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="33" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B59" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C59" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D59" s="33" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -8587,86 +8584,86 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="33" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B61" s="36" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C61" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D61" s="33" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="32" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B62" s="39" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C62" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D62" s="32" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="33" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B63" s="33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C63" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D63" s="33" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="32" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B64" s="32" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C64" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D64" s="32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="33" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B65" s="33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C65" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D65" s="33" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="32" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B66" s="32" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C66" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D66" s="32" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -8687,44 +8684,44 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="33" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B69" s="33" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C69" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D69" s="33" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="32" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B70" s="32" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C70" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D70" s="32" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="33" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B71" s="33" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C71" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D71" s="33" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>